<commit_message>
three apis merged in single one
</commit_message>
<xml_diff>
--- a/myDbFiles/unavailableDevelopers.xlsx
+++ b/myDbFiles/unavailableDevelopers.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N146"/>
+  <dimension ref="A1:N147"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6406,9 +6406,50 @@
         <v>https://sourcebae.s3.amazonaws.com/staging/pdf/1655102702406.pdf</v>
       </c>
     </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>pranshu</v>
+      </c>
+      <c r="B147" t="str">
+        <v>sharma</v>
+      </c>
+      <c r="C147" t="str">
+        <v>deepak</v>
+      </c>
+      <c r="D147" t="str">
+        <v/>
+      </c>
+      <c r="E147" t="str">
+        <v>React Js</v>
+      </c>
+      <c r="F147" t="str">
+        <v>developer</v>
+      </c>
+      <c r="G147" t="str">
+        <v/>
+      </c>
+      <c r="H147">
+        <v>4</v>
+      </c>
+      <c r="I147">
+        <v>50</v>
+      </c>
+      <c r="K147" t="b">
+        <v>1</v>
+      </c>
+      <c r="L147" t="b">
+        <v>0</v>
+      </c>
+      <c r="M147">
+        <v>0</v>
+      </c>
+      <c r="N147" t="str">
+        <v>https://sourcebae.s3.amazonaws.com/staging/pdf/1655284817859.pdf</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N146"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N147"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>